<commit_message>
Add weekly checklist and PDF access sections to enhance user guidance
</commit_message>
<xml_diff>
--- a/assets/docs/budget.xlsx
+++ b/assets/docs/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8c008f664dc4ac1/Documents/Ecole/S3/ProdConMe2/Etoile_Blanche/Playbook/assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{9AA2756B-EC90-4F4F-A074-BAA045E96301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7728330E-660A-44A2-939E-CB8BB4128FEA}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{9AA2756B-EC90-4F4F-A074-BAA045E96301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D662D31-8DE8-412F-951B-77B62A2D24A5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6F22DEA2-3518-4CCD-A064-B2603ED29C95}"/>
   </bookViews>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00386C9C-14EB-4C12-BF83-592E97415448}">
-  <dimension ref="A2:F22"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,33 +757,36 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D21" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="13"/>
+      <c r="B22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="7">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="8" t="s">
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
-        <f>SUM(E5,E13,E21)</f>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <f>SUM(E5,E13,E22)</f>
         <v>1413</v>
       </c>
     </row>
@@ -791,7 +794,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="A14:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add design rules and specifications for menu cards in HTML
</commit_message>
<xml_diff>
--- a/assets/docs/budget.xlsx
+++ b/assets/docs/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8c008f664dc4ac1/Documents/Ecole/S3/ProdConMe2/Etoile_Blanche/Playbook/assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{9AA2756B-EC90-4F4F-A074-BAA045E96301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D662D31-8DE8-412F-951B-77B62A2D24A5}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{9AA2756B-EC90-4F4F-A074-BAA045E96301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{829358AD-5F78-4AE0-BE99-4F57606DC179}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6F22DEA2-3518-4CCD-A064-B2603ED29C95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Glaçons</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pinces métalliques (Amazon/Aliexpress, 30 pièces) </t>
+  </si>
+  <si>
+    <t>Supports Stand-Up (20 pièces)</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,6 +760,12 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>

</xml_diff>

<commit_message>
feat: Update budget estimates and add new line item in index.html
</commit_message>
<xml_diff>
--- a/assets/docs/budget.xlsx
+++ b/assets/docs/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8c008f664dc4ac1/Documents/Ecole/S3/ProdConMe2/Etoile_Blanche/Playbook/assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{9AA2756B-EC90-4F4F-A074-BAA045E96301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{829358AD-5F78-4AE0-BE99-4F57606DC179}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{9AA2756B-EC90-4F4F-A074-BAA045E96301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36FB4278-8856-4FAA-9A37-5281C8026A4C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6F22DEA2-3518-4CCD-A064-B2603ED29C95}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +784,8 @@
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="7">
-        <v>179</v>
+        <f>SUM(D19:D21)</f>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -796,7 +797,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7">
         <f>SUM(E5,E13,E22)</f>
-        <v>1413</v>
+        <v>1463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>